<commit_message>
+= update get debit detail ar sum
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_DebitDetail_Template.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.ReportData/eFMS.API.ReportData/FormatExcel/TemplateExport/AccountReceivable/AR_DebitDetail_Template.xlsx
@@ -1,30 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\eFMS-WebApp\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\eFMS\WebAPI\eFMS.API.SystemWeb\eFMS.API.ReportData\eFMS.API.ReportData\FormatExcel\TemplateExport\AccountReceivable\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A5FC83C-DD7B-4C83-A949-6A3EC3CF2500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4050" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>No</t>
   </si>
@@ -114,12 +123,24 @@
   </si>
   <si>
     <t>Debit Detail - {DebitType}</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Salesman</t>
+  </si>
+  <si>
+    <t>{Services}</t>
+  </si>
+  <si>
+    <t>{Salesman}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
@@ -212,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -235,10 +256,16 @@
     <xf numFmtId="43" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,20 +562,20 @@
     <col min="6" max="7" width="17.140625" customWidth="1"/>
     <col min="8" max="8" width="16.85546875" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" customWidth="1"/>
-    <col min="10" max="10" width="16.42578125" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" customWidth="1"/>
-    <col min="12" max="12" width="12.5703125" customWidth="1"/>
-    <col min="13" max="13" width="14.28515625" customWidth="1"/>
-    <col min="14" max="14" width="21" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="12" width="16.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.85546875" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.28515625" customWidth="1"/>
+    <col min="16" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="E1" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -579,20 +606,26 @@
       <c r="J3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="L3" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="N3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M3" s="6" t="s">
+      <c r="O3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="P3" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>15</v>
       </c>
@@ -623,21 +656,27 @@
       <c r="J4" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="K4" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="L4" s="5" t="s">
+      <c r="N4" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="P4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O4" s="17"/>
+      <c r="Q4" s="16"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -648,18 +687,20 @@
       <c r="H5" s="8"/>
       <c r="I5" s="4"/>
       <c r="J5" s="8"/>
-      <c r="K5" s="1"/>
-      <c r="L5" s="5"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
       <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="16"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="17"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
       <c r="E6" s="11">
         <f>SUM(E4:E5)</f>
         <v>0</v>
@@ -684,10 +725,12 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
       <c r="M6" s="7"/>
       <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -699,6 +742,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006FD60B2B3B61EC4B818F80CD946D5E28" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e5742b39f54ecbf7a248700020ef6d10">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cc0f44bc-12c1-426c-9c9e-31369e27d6a3" xmlns:ns4="702a5875-706b-4aaa-920b-b6d492c17630" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d1bddb5d083f4db09295017e397ee70" ns3:_="" ns4:_="">
     <xsd:import namespace="cc0f44bc-12c1-426c-9c9e-31369e27d6a3"/>
@@ -895,22 +953,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F4E6D7-2173-4855-B72E-B454B205DDA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F66DAAF6-2D09-4A7A-98BC-D382A08213D3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="702a5875-706b-4aaa-920b-b6d492c17630"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="cc0f44bc-12c1-426c-9c9e-31369e27d6a3"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8261FAC-87D0-44F1-97E6-B21C0FEAE03C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -927,29 +995,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F66DAAF6-2D09-4A7A-98BC-D382A08213D3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="702a5875-706b-4aaa-920b-b6d492c17630"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="cc0f44bc-12c1-426c-9c9e-31369e27d6a3"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19F4E6D7-2173-4855-B72E-B454B205DDA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>